<commit_message>
Added file warnings, reject password file, other changes
</commit_message>
<xml_diff>
--- a/FileObjectExtractorTests/Resources/TestExcel.xlsx
+++ b/FileObjectExtractorTests/Resources/TestExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\source\repos\FileObjectExtractor\FileObjectExtractorTests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C0DC16-383D-4DC6-B21A-B7F03238C64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5E7E13-2EA4-49F7-869C-47450CF4D099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,35 +407,30 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>3</xdr:row>
+          <xdr:row>30</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="Object 1" hidden="1">
+            <xdr:cNvPr id="1033" name="Object 9" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2049"/>
+                  <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAA13200-FF08-8836-B3F3-D1D3E2DB2EB7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB45FA2C-29FE-553D-473C-E34271EEE605}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -473,6 +468,121 @@
                 </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>304800</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>390525</xdr:colOff>
+          <xdr:row>39</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2050" name="Object 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -748,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,6 +1019,31 @@
         <oleObject progId="Document" shapeId="1032" r:id="rId14"/>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Bitmap Image" dvAspect="DVASPECT_ICON" shapeId="1033" r:id="rId16">
+          <objectPr defaultSize="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>304800</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Bitmap Image" dvAspect="DVASPECT_ICON" shapeId="1033" r:id="rId16"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
 </worksheet>
 </file>
@@ -917,37 +1052,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24034A34-B244-4E92-9691-FB6ED083F061}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Acrobat Document" dvAspect="DVASPECT_ICON" shapeId="2049" r:id="rId3">
-          <objectPr defaultSize="0" r:id="rId4">
+        <oleObject progId="Acrobat Document" dvAspect="DVASPECT_ICON" shapeId="2049" r:id="rId4">
+          <objectPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>304800</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Acrobat Document" dvAspect="DVASPECT_ICON" shapeId="2049" r:id="rId3"/>
+        <oleObject progId="Acrobat Document" dvAspect="DVASPECT_ICON" shapeId="2049" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Document" shapeId="2050" r:id="rId6">
+          <objectPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>142875</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>390525</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Document" shapeId="2050" r:id="rId6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>